<commit_message>
records json first cut
</commit_message>
<xml_diff>
--- a/owlcms/src/test/resources/testData/records/EWFRecords.xlsx
+++ b/owlcms/src/test/resources/testData/records/EWFRecords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms4\owlcms\src\test\resources\testData\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08BAA1C-1DCE-4D16-8554-5F083DA6C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC40ED1D-BB1D-4428-AADC-B5F66BDF49E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{DF28E3F7-8829-40AC-8AE2-BA2E1FA35BEA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DF28E3F7-8829-40AC-8AE2-BA2E1FA35BEA}"/>
   </bookViews>
   <sheets>
     <sheet name="EWF SR M" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="99">
   <si>
     <t>bwcat</t>
   </si>
@@ -323,6 +323,18 @@
   </si>
   <si>
     <t>Moscow-RUS</t>
+  </si>
+  <si>
+    <t>&gt;81</t>
+  </si>
+  <si>
+    <t>&gt;102</t>
+  </si>
+  <si>
+    <t>&gt;87</t>
+  </si>
+  <si>
+    <t>&gt;109</t>
   </si>
 </sst>
 </file>
@@ -752,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3A71D5-0912-46D0-92EA-6C23C6C08BFF}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,8 +1998,8 @@
       <c r="G29" s="3">
         <v>109</v>
       </c>
-      <c r="H29" s="3">
-        <v>999</v>
+      <c r="H29" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>11</v>
@@ -2033,8 +2045,8 @@
       <c r="G30" s="3">
         <v>109</v>
       </c>
-      <c r="H30" s="3">
-        <v>999</v>
+      <c r="H30" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>13</v>
@@ -2080,8 +2092,8 @@
       <c r="G31" s="3">
         <v>109</v>
       </c>
-      <c r="H31" s="3">
-        <v>999</v>
+      <c r="H31" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>14</v>
@@ -2115,7 +2127,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="H30" sqref="H30:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3342,8 +3354,8 @@
       <c r="G29" s="3">
         <v>87</v>
       </c>
-      <c r="H29" s="3">
-        <v>999</v>
+      <c r="H29" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>11</v>
@@ -3389,8 +3401,8 @@
       <c r="G30" s="3">
         <v>87</v>
       </c>
-      <c r="H30" s="3">
-        <v>999</v>
+      <c r="H30" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>13</v>
@@ -3436,8 +3448,8 @@
       <c r="G31" s="3">
         <v>87</v>
       </c>
-      <c r="H31" s="3">
-        <v>999</v>
+      <c r="H31" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>14</v>
@@ -3472,7 +3484,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="H30" sqref="H30:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5088,8 +5100,8 @@
       <c r="G29" s="3">
         <v>109</v>
       </c>
-      <c r="H29">
-        <v>999</v>
+      <c r="H29" t="s">
+        <v>98</v>
       </c>
       <c r="I29" t="s">
         <v>11</v>
@@ -5148,8 +5160,8 @@
       <c r="G30" s="3">
         <v>109</v>
       </c>
-      <c r="H30">
-        <v>999</v>
+      <c r="H30" t="s">
+        <v>98</v>
       </c>
       <c r="I30" t="s">
         <v>13</v>
@@ -5199,8 +5211,8 @@
       <c r="G31" s="3">
         <v>109</v>
       </c>
-      <c r="H31">
-        <v>999</v>
+      <c r="H31" t="s">
+        <v>98</v>
       </c>
       <c r="I31" t="s">
         <v>14</v>
@@ -5247,7 +5259,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="H30" sqref="H30:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6453,8 +6465,8 @@
       <c r="G29" s="3">
         <v>87</v>
       </c>
-      <c r="H29" s="3">
-        <v>999</v>
+      <c r="H29" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>11</v>
@@ -6493,8 +6505,8 @@
       <c r="G30" s="3">
         <v>87</v>
       </c>
-      <c r="H30" s="3">
-        <v>999</v>
+      <c r="H30" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>13</v>
@@ -6533,8 +6545,8 @@
       <c r="G31" s="3">
         <v>87</v>
       </c>
-      <c r="H31" s="3">
-        <v>999</v>
+      <c r="H31" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>14</v>
@@ -6561,7 +6573,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="H30" sqref="H30:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7860,8 +7872,8 @@
       <c r="G29" s="3">
         <v>102</v>
       </c>
-      <c r="H29" s="17">
-        <v>999</v>
+      <c r="H29" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>11</v>
@@ -7901,8 +7913,8 @@
       <c r="G30" s="3">
         <v>102</v>
       </c>
-      <c r="H30" s="17">
-        <v>999</v>
+      <c r="H30" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>13</v>
@@ -7942,8 +7954,8 @@
       <c r="G31" s="3">
         <v>102</v>
       </c>
-      <c r="H31" s="17">
-        <v>999</v>
+      <c r="H31" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>14</v>
@@ -7981,8 +7993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C3D9D4-F036-48B2-893F-5441C8E76D19}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9263,8 +9275,8 @@
       <c r="G29" s="3">
         <v>81</v>
       </c>
-      <c r="H29" s="3">
-        <v>999</v>
+      <c r="H29" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>11</v>
@@ -9304,8 +9316,8 @@
       <c r="G30" s="3">
         <v>81</v>
       </c>
-      <c r="H30" s="3">
-        <v>999</v>
+      <c r="H30" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>13</v>
@@ -9345,8 +9357,8 @@
       <c r="G31" s="3">
         <v>81</v>
       </c>
-      <c r="H31" s="3">
-        <v>999</v>
+      <c r="H31" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>14</v>

</xml_diff>